<commit_message>
recoding, imc, pression arterielle.
</commit_message>
<xml_diff>
--- a/Dictionnaire.xlsx
+++ b/Dictionnaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dr Calixte Assogba\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELITEBOOK 1030 G2\Desktop\HTA_VIH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A8F6A2-B65A-4F4A-A73D-E0D2D017F55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5042988C-0562-4920-AF31-629BE4104817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D56E12D5-E170-43F6-854E-16EE419504EE}"/>
+    <workbookView xWindow="9720" yWindow="490" windowWidth="9480" windowHeight="9570" xr2:uid="{D56E12D5-E170-43F6-854E-16EE419504EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="245">
   <si>
     <t>MNT_odk-Welcome</t>
   </si>
@@ -534,16 +534,257 @@
   </si>
   <si>
     <t>Creatinine</t>
+  </si>
+  <si>
+    <t>id_depart</t>
+  </si>
+  <si>
+    <t>centre</t>
+  </si>
+  <si>
+    <t>id_enq</t>
+  </si>
+  <si>
+    <t>num_enr</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>sexe</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>ethnie</t>
+  </si>
+  <si>
+    <t>tabagisme</t>
+  </si>
+  <si>
+    <t>niv_instr</t>
+  </si>
+  <si>
+    <t>etat_civil</t>
+  </si>
+  <si>
+    <t>ctg_sociopro</t>
+  </si>
+  <si>
+    <t>alcool</t>
+  </si>
+  <si>
+    <t>nbre_port_leg_jrs</t>
+  </si>
+  <si>
+    <t>nbre_port_fruit_jrs</t>
+  </si>
+  <si>
+    <t>freq_ajt_sel</t>
+  </si>
+  <si>
+    <t>nbre_jrs_cons_fruit</t>
+  </si>
+  <si>
+    <t>nbre_jrs_cons_leg</t>
+  </si>
+  <si>
+    <t>freq_cons_plat_sel</t>
+  </si>
+  <si>
+    <t>act_phsq_travail</t>
+  </si>
+  <si>
+    <t>act_phsq_dpl</t>
+  </si>
+  <si>
+    <t>ant_hta</t>
+  </si>
+  <si>
+    <t>trat_mod_hta</t>
+  </si>
+  <si>
+    <t>trat_trad_hta</t>
+  </si>
+  <si>
+    <t>ant_diabete</t>
+  </si>
+  <si>
+    <t>trat_mod_diabete</t>
+  </si>
+  <si>
+    <t>trat_trad_diabete</t>
+  </si>
+  <si>
+    <t>ant_hchol</t>
+  </si>
+  <si>
+    <t>trat_mod_hchol</t>
+  </si>
+  <si>
+    <t>trat_trad_hchol</t>
+  </si>
+  <si>
+    <t>ant_card</t>
+  </si>
+  <si>
+    <t>aspir_proph</t>
+  </si>
+  <si>
+    <t>statine</t>
+  </si>
+  <si>
+    <t>depression</t>
+  </si>
+  <si>
+    <t>fatigue</t>
+  </si>
+  <si>
+    <t>dim_interet</t>
+  </si>
+  <si>
+    <t>gn_pert_pds</t>
+  </si>
+  <si>
+    <t>insm_hysm</t>
+  </si>
+  <si>
+    <t>ftg_pert_eng</t>
+  </si>
+  <si>
+    <t>devalorisation</t>
+  </si>
+  <si>
+    <t>dim_apt_penser</t>
+  </si>
+  <si>
+    <t>idee_mort</t>
+  </si>
+  <si>
+    <t>ronflement_fort</t>
+  </si>
+  <si>
+    <t>ftg_sml</t>
+  </si>
+  <si>
+    <t>arret_resp_noct</t>
+  </si>
+  <si>
+    <t>date_debut</t>
+  </si>
+  <si>
+    <t>echec_clinique</t>
+  </si>
+  <si>
+    <t>hta</t>
+  </si>
+  <si>
+    <t>tas</t>
+  </si>
+  <si>
+    <t>tad</t>
+  </si>
+  <si>
+    <t>taille</t>
+  </si>
+  <si>
+    <t>poids</t>
+  </si>
+  <si>
+    <t>glycemie</t>
+  </si>
+  <si>
+    <t>triglycerides</t>
+  </si>
+  <si>
+    <t>uree</t>
+  </si>
+  <si>
+    <t>creatinine</t>
+  </si>
+  <si>
+    <t>stde_vih</t>
+  </si>
+  <si>
+    <t>trtment_arv_1</t>
+  </si>
+  <si>
+    <t>trtment_arv_2</t>
+  </si>
+  <si>
+    <t>trtment_arv_3</t>
+  </si>
+  <si>
+    <t>trtment_arv_4</t>
+  </si>
+  <si>
+    <t>trtment_arv_5</t>
+  </si>
+  <si>
+    <t>echec_imun</t>
+  </si>
+  <si>
+    <t>echec_virol</t>
+  </si>
+  <si>
+    <t>ext_exm_paracl</t>
+  </si>
+  <si>
+    <t>chl_total</t>
+  </si>
+  <si>
+    <t>chl_hdl</t>
+  </si>
+  <si>
+    <t>chl_ldl</t>
+  </si>
+  <si>
+    <t>act_phsq_loisir</t>
+  </si>
+  <si>
+    <t>duree_ass_couch_jr</t>
+  </si>
+  <si>
+    <t>agt_rlt_psych</t>
+  </si>
+  <si>
+    <t>tour_cou_imp</t>
+  </si>
+  <si>
+    <t>enceinte</t>
+  </si>
+  <si>
+    <t>tour_taille</t>
+  </si>
+  <si>
+    <t>tour_hanche</t>
+  </si>
+  <si>
+    <t>an_depsg</t>
+  </si>
+  <si>
+    <t>dte_realisation</t>
+  </si>
+  <si>
+    <t>hgb_glyquee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -569,9 +810,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -888,750 +1130,987 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{040548E3-7FB2-4699-8D76-5AB722764E9A}">
   <dimension ref="A1:CD91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" customWidth="1"/>
-    <col min="2" max="2" width="42.77734375" customWidth="1"/>
-    <col min="3" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.90625" customWidth="1"/>
+    <col min="2" max="2" width="41.36328125" customWidth="1"/>
+    <col min="3" max="4" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="31.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="23" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="36.36328125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="18" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="36.36328125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="18" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="36.36328125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="36.36328125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="18" bestFit="1" customWidth="1"/>
     <col min="34" max="36" width="17" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="40" max="42" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="43" max="45" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="54" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="56" max="60" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="62" max="63" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="64" max="69" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="71" max="73" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="74" max="77" width="13.6640625" customWidth="1"/>
-    <col min="78" max="80" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="83" max="89" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="40" max="42" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="45" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="46" max="54" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="56" max="60" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="62" max="63" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="64" max="69" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="71" max="73" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="74" max="77" width="13.6328125" customWidth="1"/>
+    <col min="78" max="80" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="83" max="89" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="40.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="C13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="C16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="C18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="C25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="C27" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="C29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="C31" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="C60" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>68</v>
       </c>
       <c r="B69" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>90</v>
       </c>
       <c r="B71" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C71" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>70</v>
       </c>
       <c r="B72" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>85</v>
       </c>
       <c r="B73" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>86</v>
       </c>
       <c r="B74" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>87</v>
       </c>
       <c r="B75" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>88</v>
       </c>
       <c r="B76" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>89</v>
       </c>
       <c r="B77" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>71</v>
       </c>
       <c r="B78" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>72</v>
       </c>
       <c r="B79" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>73</v>
       </c>
       <c r="B80" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C80" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>74</v>
       </c>
       <c r="B81" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C81" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B82" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C82" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>76</v>
       </c>
       <c r="B83" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C83" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>77</v>
       </c>
       <c r="B84" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C84" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>78</v>
       </c>
       <c r="B85" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C85" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>79</v>
       </c>
       <c r="B86" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C86" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>80</v>
       </c>
       <c r="B87" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C87" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>81</v>
       </c>
       <c r="B88" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C88" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>82</v>
       </c>
       <c r="B89" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C89" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>83</v>
       </c>
       <c r="B90" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+      <c r="C90" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="2" t="s">
         <v>84</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>